<commit_message>
Com Acre e Amapá
</commit_message>
<xml_diff>
--- a/dadosTeste.xlsx
+++ b/dadosTeste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francisco/Dropbox/Estudos/Data/Python/Environments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFF0650-DDCB-7847-890E-DE27938BB3F1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84931390-53A9-894E-9648-7E0E0ED100F0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="460" windowWidth="25860" windowHeight="16340" xr2:uid="{2184D749-8611-904A-ABE6-4596C639FEE6}"/>
+    <workbookView xWindow="360" yWindow="460" windowWidth="34420" windowHeight="16340" activeTab="5" xr2:uid="{2184D749-8611-904A-ABE6-4596C639FEE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Compilado" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="142">
   <si>
     <t>UF</t>
   </si>
@@ -1338,22 +1338,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="40" fontId="19" fillId="0" borderId="31" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="40" fontId="19" fillId="0" borderId="32" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="40" fontId="19" fillId="0" borderId="18" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="40" fontId="19" fillId="5" borderId="26" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="40" fontId="14" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="40" fontId="19" fillId="5" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="17" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="40" fontId="18" fillId="0" borderId="25" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1377,13 +1368,22 @@
     <xf numFmtId="40" fontId="17" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="40" fontId="14" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="40" fontId="19" fillId="0" borderId="31" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="40" fontId="19" fillId="0" borderId="32" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="40" fontId="19" fillId="0" borderId="18" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="40" fontId="19" fillId="5" borderId="26" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="17" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="40" fontId="19" fillId="5" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1815,8 +1815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382335A9-A7F8-2F4A-87B2-B1443864BF02}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1856,12 +1856,12 @@
         <v>176289423.88999999</v>
       </c>
       <c r="D2" s="1">
-        <f>SUM(Recursos173!B2:F2)</f>
-        <v>0</v>
+        <f>SUM(Recursos173!B2:G2)</f>
+        <v>112741576.54000001</v>
       </c>
       <c r="E2" s="5">
-        <f>SUM(Suspensao173!B2:F2)</f>
-        <v>5294537.34</v>
+        <f>SUM(Suspensao173!B2:G2)</f>
+        <v>7059383.1200000001</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1916,12 +1916,12 @@
         <v>162252603.16000003</v>
       </c>
       <c r="D5" s="1">
-        <f>SUM(Recursos173!B5:F5)</f>
-        <v>0</v>
+        <f>SUM(Recursos173!B5:G5)</f>
+        <v>133547895.78</v>
       </c>
       <c r="E5" s="5">
-        <f>SUM(Suspensao173!B5:F5)</f>
-        <v>1972974.75</v>
+        <f>SUM(Suspensao173!B5:G5)</f>
+        <v>2630633</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2397,11 +2397,11 @@
       </c>
       <c r="D29" s="5">
         <f>SUM(D2:D28)</f>
-        <v>9003710527.6800022</v>
+        <v>9250000000.0000019</v>
       </c>
       <c r="E29" s="5">
         <f>SUM(E2:E28)</f>
-        <v>6173419101.0100002</v>
+        <v>6175841605.04</v>
       </c>
     </row>
   </sheetData>
@@ -2434,16 +2434,16 @@
       <c r="D1" s="65"/>
     </row>
     <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.15">
-      <c r="A2" s="113" t="s">
+      <c r="A2" s="100" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="113"/>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B3" s="114"/>
-      <c r="C3" s="114"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
       <c r="D3" s="65"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
@@ -2454,25 +2454,25 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="115"/>
-      <c r="B5" s="106" t="s">
+      <c r="A5" s="102"/>
+      <c r="B5" s="103" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="107" t="s">
+      <c r="C5" s="104" t="s">
         <v>85</v>
       </c>
-      <c r="D5" s="107" t="s">
+      <c r="D5" s="104" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="115"/>
-      <c r="B6" s="106"/>
-      <c r="C6" s="107"/>
-      <c r="D6" s="107"/>
+      <c r="A6" s="102"/>
+      <c r="B6" s="103"/>
+      <c r="C6" s="104"/>
+      <c r="D6" s="104"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" s="108" t="s">
+      <c r="A7" s="105" t="s">
         <v>87</v>
       </c>
       <c r="B7" s="70" t="s">
@@ -2493,7 +2493,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="108"/>
+      <c r="A8" s="105"/>
       <c r="B8" s="70" t="s">
         <v>89</v>
       </c>
@@ -2512,7 +2512,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" s="108"/>
+      <c r="A9" s="105"/>
       <c r="B9" s="70" t="s">
         <v>90</v>
       </c>
@@ -2531,7 +2531,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="108"/>
+      <c r="A10" s="105"/>
       <c r="B10" s="70" t="s">
         <v>91</v>
       </c>
@@ -2550,7 +2550,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11" s="108"/>
+      <c r="A11" s="105"/>
       <c r="B11" s="70" t="s">
         <v>92</v>
       </c>
@@ -2569,7 +2569,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" s="108"/>
+      <c r="A12" s="105"/>
       <c r="B12" s="70" t="s">
         <v>93</v>
       </c>
@@ -2588,7 +2588,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A13" s="108"/>
+      <c r="A13" s="105"/>
       <c r="B13" s="70" t="s">
         <v>94</v>
       </c>
@@ -2607,7 +2607,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A14" s="108"/>
+      <c r="A14" s="105"/>
       <c r="B14" s="70" t="s">
         <v>95</v>
       </c>
@@ -2626,7 +2626,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A15" s="108"/>
+      <c r="A15" s="105"/>
       <c r="B15" s="70" t="s">
         <v>96</v>
       </c>
@@ -2645,7 +2645,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A16" s="108"/>
+      <c r="A16" s="105"/>
       <c r="B16" s="70" t="s">
         <v>97</v>
       </c>
@@ -2664,7 +2664,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A17" s="108"/>
+      <c r="A17" s="105"/>
       <c r="B17" s="70" t="s">
         <v>98</v>
       </c>
@@ -2683,7 +2683,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A18" s="108"/>
+      <c r="A18" s="105"/>
       <c r="B18" s="70" t="s">
         <v>99</v>
       </c>
@@ -2702,7 +2702,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A19" s="108"/>
+      <c r="A19" s="105"/>
       <c r="B19" s="70" t="s">
         <v>100</v>
       </c>
@@ -2721,7 +2721,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A20" s="108"/>
+      <c r="A20" s="105"/>
       <c r="B20" s="70" t="s">
         <v>101</v>
       </c>
@@ -2740,7 +2740,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A21" s="108"/>
+      <c r="A21" s="105"/>
       <c r="B21" s="70" t="s">
         <v>102</v>
       </c>
@@ -2759,7 +2759,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A22" s="108"/>
+      <c r="A22" s="105"/>
       <c r="B22" s="70" t="s">
         <v>103</v>
       </c>
@@ -2778,7 +2778,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A23" s="108"/>
+      <c r="A23" s="105"/>
       <c r="B23" s="70" t="s">
         <v>104</v>
       </c>
@@ -2797,7 +2797,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A24" s="108"/>
+      <c r="A24" s="105"/>
       <c r="B24" s="70" t="s">
         <v>105</v>
       </c>
@@ -2816,7 +2816,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A25" s="108"/>
+      <c r="A25" s="105"/>
       <c r="B25" s="70" t="s">
         <v>106</v>
       </c>
@@ -2835,7 +2835,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A26" s="108"/>
+      <c r="A26" s="105"/>
       <c r="B26" s="70" t="s">
         <v>107</v>
       </c>
@@ -2854,7 +2854,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A27" s="108"/>
+      <c r="A27" s="105"/>
       <c r="B27" s="70" t="s">
         <v>108</v>
       </c>
@@ -2873,7 +2873,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A28" s="108"/>
+      <c r="A28" s="105"/>
       <c r="B28" s="73" t="s">
         <v>109</v>
       </c>
@@ -2885,7 +2885,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A29" s="109" t="s">
+      <c r="A29" s="106" t="s">
         <v>110</v>
       </c>
       <c r="B29" s="70" t="s">
@@ -2899,7 +2899,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A30" s="109"/>
+      <c r="A30" s="106"/>
       <c r="B30" s="70" t="s">
         <v>112</v>
       </c>
@@ -2911,7 +2911,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A31" s="109"/>
+      <c r="A31" s="106"/>
       <c r="B31" s="70" t="s">
         <v>113</v>
       </c>
@@ -2923,7 +2923,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A32" s="109"/>
+      <c r="A32" s="106"/>
       <c r="B32" s="75" t="s">
         <v>114</v>
       </c>
@@ -2949,10 +2949,10 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="110" t="s">
+      <c r="A34" s="107" t="s">
         <v>117</v>
       </c>
-      <c r="B34" s="110"/>
+      <c r="B34" s="107"/>
       <c r="C34" s="76">
         <v>2901326.2360000005</v>
       </c>
@@ -2961,21 +2961,21 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B35" s="111" t="s">
+      <c r="B35" s="108" t="s">
         <v>118</v>
       </c>
-      <c r="C35" s="111"/>
-      <c r="D35" s="111"/>
+      <c r="C35" s="108"/>
+      <c r="D35" s="108"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B36" s="112"/>
-      <c r="C36" s="112"/>
-      <c r="D36" s="112"/>
+      <c r="B36" s="109"/>
+      <c r="C36" s="109"/>
+      <c r="D36" s="109"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B37" s="112"/>
-      <c r="C37" s="112"/>
-      <c r="D37" s="112"/>
+      <c r="B37" s="109"/>
+      <c r="C37" s="109"/>
+      <c r="D37" s="109"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D38" s="69" t="s">
@@ -2983,23 +2983,23 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B39" s="106" t="s">
+      <c r="B39" s="103" t="s">
         <v>119</v>
       </c>
-      <c r="C39" s="107" t="s">
+      <c r="C39" s="104" t="s">
         <v>85</v>
       </c>
-      <c r="D39" s="107" t="s">
+      <c r="D39" s="104" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B40" s="106"/>
-      <c r="C40" s="107"/>
-      <c r="D40" s="107"/>
+      <c r="B40" s="103"/>
+      <c r="C40" s="104"/>
+      <c r="D40" s="104"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="101" t="s">
+      <c r="A41" s="111" t="s">
         <v>87</v>
       </c>
       <c r="B41" s="70" t="s">
@@ -3013,7 +3013,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A42" s="102"/>
+      <c r="A42" s="112"/>
       <c r="B42" s="70" t="s">
         <v>121</v>
       </c>
@@ -3025,7 +3025,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="103"/>
+      <c r="A43" s="113"/>
       <c r="B43" s="70" t="s">
         <v>122</v>
       </c>
@@ -3037,10 +3037,10 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="104" t="s">
+      <c r="A44" s="114" t="s">
         <v>117</v>
       </c>
-      <c r="B44" s="105"/>
+      <c r="B44" s="115"/>
       <c r="C44" s="79">
         <v>270630.40295999998</v>
       </c>
@@ -3062,21 +3062,21 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B47" s="106" t="s">
+      <c r="B47" s="103" t="s">
         <v>123</v>
       </c>
-      <c r="C47" s="107" t="s">
+      <c r="C47" s="104" t="s">
         <v>85</v>
       </c>
-      <c r="D47" s="107" t="s">
+      <c r="D47" s="104" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A48" s="82"/>
-      <c r="B48" s="106"/>
-      <c r="C48" s="107"/>
-      <c r="D48" s="107"/>
+      <c r="B48" s="103"/>
+      <c r="C48" s="104"/>
+      <c r="D48" s="104"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B49" s="83" t="s">
@@ -3138,38 +3138,38 @@
       <c r="D54" s="89"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="100" t="s">
+      <c r="A55" s="110" t="s">
         <v>127</v>
       </c>
-      <c r="B55" s="100"/>
-      <c r="C55" s="100"/>
-      <c r="D55" s="100"/>
+      <c r="B55" s="110"/>
+      <c r="C55" s="110"/>
+      <c r="D55" s="110"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="100"/>
-      <c r="B56" s="100"/>
-      <c r="C56" s="100"/>
-      <c r="D56" s="100"/>
+      <c r="A56" s="110"/>
+      <c r="B56" s="110"/>
+      <c r="C56" s="110"/>
+      <c r="D56" s="110"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="100"/>
-      <c r="B57" s="100"/>
-      <c r="C57" s="100"/>
-      <c r="D57" s="100"/>
+      <c r="A57" s="110"/>
+      <c r="B57" s="110"/>
+      <c r="C57" s="110"/>
+      <c r="D57" s="110"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A58" s="100" t="s">
+      <c r="A58" s="110" t="s">
         <v>128</v>
       </c>
-      <c r="B58" s="100"/>
-      <c r="C58" s="100"/>
-      <c r="D58" s="100"/>
+      <c r="B58" s="110"/>
+      <c r="C58" s="110"/>
+      <c r="D58" s="110"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A59" s="100"/>
-      <c r="B59" s="100"/>
-      <c r="C59" s="100"/>
-      <c r="D59" s="100"/>
+      <c r="A59" s="110"/>
+      <c r="B59" s="110"/>
+      <c r="C59" s="110"/>
+      <c r="D59" s="110"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A60" s="82"/>
@@ -4497,12 +4497,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="A58:D59"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="A55:D57"/>
     <mergeCell ref="A7:A28"/>
     <mergeCell ref="A29:A32"/>
     <mergeCell ref="A34:B34"/>
@@ -4510,13 +4511,12 @@
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="C39:C40"/>
     <mergeCell ref="D39:D40"/>
-    <mergeCell ref="A58:D59"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="A55:D57"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -5835,7 +5835,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:G27"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7583,10 +7583,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAC27665-77EE-FE4C-B0B2-732245FB6E34}">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="B2:F2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G29" sqref="B29:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7600,7 +7600,7 @@
     <col min="12" max="13" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7641,7 +7641,7 @@
         <v>43983</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
@@ -7660,7 +7660,9 @@
       <c r="F2" s="4">
         <v>98589827.640000001</v>
       </c>
-      <c r="G2" s="4"/>
+      <c r="G2" s="4">
+        <v>100955375.23</v>
+      </c>
       <c r="H2" s="4">
         <v>120702424.48999999</v>
       </c>
@@ -7676,8 +7678,14 @@
       <c r="L2" s="4">
         <v>77434978.8699999</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M2" s="4">
+        <v>89821973.030000001</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
@@ -7717,8 +7725,11 @@
       <c r="M3" s="4">
         <v>298637470.19999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -7758,8 +7769,11 @@
       <c r="M4">
         <v>798202512.34000003</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -7778,7 +7792,9 @@
       <c r="F5" s="4">
         <v>68756590.230000004</v>
       </c>
-      <c r="G5" s="4"/>
+      <c r="G5" s="4">
+        <v>73070197.530000001</v>
+      </c>
       <c r="H5" s="4">
         <v>86074324.319999993</v>
       </c>
@@ -7794,8 +7810,14 @@
       <c r="L5" s="4">
         <v>52305798.669999897</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M5" s="10">
+        <v>56868606.710000001</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>13</v>
       </c>
@@ -7835,8 +7857,11 @@
       <c r="M6" s="4">
         <v>1754052873.1699901</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N6" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
@@ -7876,8 +7901,11 @@
       <c r="M7" s="4">
         <v>845614222.53999996</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N7" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
@@ -7912,13 +7940,16 @@
         <v>555825044.47000003</v>
       </c>
       <c r="L8" s="4">
-        <v>544112736.79999995</v>
+        <v>545432784.48000002</v>
       </c>
       <c r="M8" s="10">
-        <v>623213822.05999994</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+        <v>625573875.10999894</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
@@ -7958,8 +7989,11 @@
       <c r="M9" s="10">
         <v>870931250.65999997</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N9" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>16</v>
       </c>
@@ -7999,8 +8033,11 @@
       <c r="M10">
         <v>1411805869.9400001</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N10" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>17</v>
       </c>
@@ -8040,8 +8077,11 @@
       <c r="M11">
         <v>524790786.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N11" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>18</v>
       </c>
@@ -8081,8 +8121,11 @@
       <c r="M12" s="4">
         <v>3780569709</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N12" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>19</v>
       </c>
@@ -8122,8 +8165,11 @@
       <c r="M13">
         <v>840090869.53999996</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N13" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>20</v>
       </c>
@@ -8163,8 +8209,11 @@
       <c r="M14">
         <v>1137697849.3199999</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N14" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>21</v>
       </c>
@@ -8204,8 +8253,11 @@
       <c r="M15" s="4">
         <v>958345947</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N15" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>22</v>
       </c>
@@ -8245,8 +8297,11 @@
       <c r="M16">
         <v>440693564.87</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N16" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>23</v>
       </c>
@@ -8286,8 +8341,11 @@
       <c r="M17">
         <v>1181739896.71</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N17" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>24</v>
       </c>
@@ -8327,8 +8385,11 @@
       <c r="M18" s="4">
         <v>356691847.86000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N18" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>25</v>
       </c>
@@ -8368,8 +8429,11 @@
       <c r="M19">
         <v>2230057290.6599998</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N19" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>26</v>
       </c>
@@ -8409,8 +8473,11 @@
       <c r="M20">
         <v>2460055379.1500001</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N20" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>27</v>
       </c>
@@ -8450,8 +8517,11 @@
       <c r="M21">
         <v>381069318.49000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N21" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>28</v>
       </c>
@@ -8491,8 +8561,11 @@
       <c r="M22" s="10">
         <v>324105648.08999997</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N22" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>29</v>
       </c>
@@ -8532,8 +8605,11 @@
       <c r="M23" s="10">
         <v>92020557.059999898</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N23" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>30</v>
       </c>
@@ -8573,8 +8649,11 @@
       <c r="M24">
         <v>2454386207.1399999</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N24" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>31</v>
       </c>
@@ -8614,8 +8693,11 @@
       <c r="M25">
         <v>1571214555.01</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N25" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>32</v>
       </c>
@@ -8655,8 +8737,11 @@
       <c r="M26">
         <v>246627174</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N26" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>2</v>
       </c>
@@ -8696,8 +8781,11 @@
       <c r="M27" s="10">
         <v>10213799925.290001</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N27" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>33</v>
       </c>
@@ -8737,8 +8825,11 @@
       <c r="M28" s="10">
         <v>248344667.38999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N28" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>59</v>
       </c>
@@ -8764,7 +8855,7 @@
       </c>
       <c r="G29" s="4">
         <f t="shared" si="0"/>
-        <v>39765039415.139999</v>
+        <v>39939064987.899994</v>
       </c>
       <c r="H29" s="4">
         <f t="shared" si="0"/>
@@ -8784,17 +8875,20 @@
       </c>
       <c r="L29" s="4">
         <f t="shared" si="0"/>
-        <v>31509572024.340004</v>
+        <v>31510892072.020004</v>
       </c>
       <c r="M29" s="4">
         <f t="shared" si="0"/>
-        <v>36044759213.98999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+        <v>36193809846.779999</v>
+      </c>
+      <c r="N29" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F30" s="9"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H31" s="94"/>
       <c r="I31" s="4"/>
       <c r="J31" s="93"/>
@@ -8802,7 +8896,7 @@
       <c r="L31" s="93"/>
       <c r="M31" s="93"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B32" s="9"/>
       <c r="H32" s="9"/>
       <c r="J32" s="9"/>
@@ -8820,9 +8914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FDEAEC8-5529-0B44-A039-A8078F138D33}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8910,7 +9002,9 @@
       <c r="L2" s="57">
         <v>6235155.7199999997</v>
       </c>
-      <c r="M2" s="4"/>
+      <c r="M2" s="4">
+        <v>7052649.3099999996</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
@@ -9031,7 +9125,9 @@
       <c r="L5" s="59">
         <v>2233089.11</v>
       </c>
-      <c r="M5" s="4"/>
+      <c r="M5" s="4">
+        <v>5502048.9100000001</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
@@ -9150,7 +9246,7 @@
         <v>168435891.84999999</v>
       </c>
       <c r="L8" s="59">
-        <v>47256659.579999998</v>
+        <v>47283183.380000003</v>
       </c>
       <c r="M8" s="4">
         <v>53751520.990000002</v>
@@ -10022,11 +10118,11 @@
       </c>
       <c r="L29" s="4">
         <f t="shared" si="0"/>
-        <v>2075931010.9899998</v>
+        <v>2075957534.79</v>
       </c>
       <c r="M29" s="4">
         <f t="shared" si="0"/>
-        <v>2594865405.5699997</v>
+        <v>2607420103.79</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
@@ -10041,8 +10137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{506999FD-8769-F640-AD20-C4D7995BDF01}">
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10098,7 +10194,7 @@
       </c>
       <c r="C2">
         <f>SUM(Compilado!D2:E2)</f>
-        <v>5294537.34</v>
+        <v>119800959.66000001</v>
       </c>
       <c r="D2" t="b">
         <f>A2=ICMS!A2</f>
@@ -10106,7 +10202,7 @@
       </c>
       <c r="E2" s="9">
         <f>0.75*SUM(ICMS!B2:G2)</f>
-        <v>406243759.58249998</v>
+        <v>481960291.005</v>
       </c>
       <c r="F2" s="9">
         <f>0.5*SUM(IPVA!B2:G2)</f>
@@ -10114,11 +10210,11 @@
       </c>
       <c r="G2" s="9">
         <f>SUM(ICMS!H2:M2)*0.75</f>
-        <v>380794571.21999991</v>
+        <v>448161050.99249995</v>
       </c>
       <c r="H2" s="9">
         <f>0.5*(SUM(IPVA!H2:M2))</f>
-        <v>16669007.419999998</v>
+        <v>20195332.074999999</v>
       </c>
       <c r="I2" t="b">
         <f>A2=IPVA!A2</f>
@@ -10126,11 +10222,11 @@
       </c>
       <c r="K2" s="93">
         <f>(H2+G2+C2)/(E2+F2)</f>
-        <v>0.94308763619890723</v>
+        <v>1.1698109363266282</v>
       </c>
       <c r="L2" s="9">
         <f>SUM(G2:H2)-SUM(E2:F2)</f>
-        <v>-29599719.107500076</v>
+        <v>-34423446.102500081</v>
       </c>
       <c r="M2" s="95"/>
     </row>
@@ -10184,7 +10280,7 @@
       <c r="P3" s="9"/>
       <c r="Q3" s="9">
         <f>SUM(H33:M34)</f>
-        <v>193782816563.40491</v>
+        <v>193901885184.7674</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -10236,7 +10332,7 @@
       <c r="N4" s="9"/>
       <c r="Q4" s="9">
         <f>SUM(B33:G34)</f>
-        <v>200938206824.22247</v>
+        <v>201068726003.79245</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -10249,7 +10345,7 @@
       </c>
       <c r="C5">
         <f>SUM(Compilado!D5:E5)</f>
-        <v>1972974.75</v>
+        <v>136178528.78</v>
       </c>
       <c r="D5" t="b">
         <f>A5=ICMS!A5</f>
@@ -10257,7 +10353,7 @@
       </c>
       <c r="E5" s="9">
         <f>0.75*(SUM(ICMS!B5:G5))</f>
-        <v>267931491.92250001</v>
+        <v>322734140.06999999</v>
       </c>
       <c r="F5" s="9">
         <f>0.5*SUM(IPVA!B5:G5)</f>
@@ -10265,11 +10361,11 @@
       </c>
       <c r="G5" s="9">
         <f>SUM(ICMS!H5:M5)*0.75</f>
-        <v>272827039.91999984</v>
+        <v>315478494.95249981</v>
       </c>
       <c r="H5" s="9">
         <f>0.5*(SUM(IPVA!H5:M5))</f>
-        <v>17835587.715</v>
+        <v>20586612.170000002</v>
       </c>
       <c r="I5" t="b">
         <f>A5=IPVA!A5</f>
@@ -10278,11 +10374,11 @@
       <c r="J5" s="9"/>
       <c r="K5" s="93">
         <f t="shared" si="0"/>
-        <v>1.00513938546996</v>
+        <v>1.3650949359431874</v>
       </c>
       <c r="L5" s="9">
         <f t="shared" si="1"/>
-        <v>-476697.53250020742</v>
+        <v>-9876866.192500174</v>
       </c>
       <c r="M5" s="95"/>
     </row>
@@ -10404,11 +10500,11 @@
       </c>
       <c r="G8" s="9">
         <f>SUM(ICMS!H8:M8)*0.75</f>
-        <v>2980537632.0075006</v>
+        <v>2983297707.5549998</v>
       </c>
       <c r="H8" s="9">
         <f>0.5*(SUM(IPVA!H8:M8))</f>
-        <v>486767336.98500001</v>
+        <v>486780598.88499999</v>
       </c>
       <c r="I8" t="b">
         <f>A8=IPVA!A8</f>
@@ -10417,11 +10513,11 @@
       <c r="J8" s="9"/>
       <c r="K8" s="93">
         <f t="shared" si="0"/>
-        <v>1.0457197031951053</v>
+        <v>1.046511017493019</v>
       </c>
       <c r="L8" s="9">
         <f t="shared" si="1"/>
-        <v>-37418065.59749651</v>
+        <v>-34644728.149997711</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -11354,7 +11450,7 @@
       </c>
       <c r="C29">
         <f>SUM(Compilado!D29:E29)</f>
-        <v>15177129628.690002</v>
+        <v>15425841605.040001</v>
       </c>
       <c r="D29" t="b">
         <f>A29=ICMS!A29</f>
@@ -11362,7 +11458,7 @@
       </c>
       <c r="E29" s="9">
         <f>0.75*(SUM(ICMS!B29:G29))</f>
-        <v>183383387226.26248</v>
+        <v>183513906405.83246</v>
       </c>
       <c r="F29" s="9">
         <f>0.5*SUM(IPVA!B29:G29)</f>
@@ -11370,11 +11466,11 @@
       </c>
       <c r="G29" s="9">
         <f>SUM(ICMS!H29:M29)*0.75</f>
-        <v>176439837101.75995</v>
+        <v>176552615112.11246</v>
       </c>
       <c r="H29" s="9">
         <f>0.5*(SUM(IPVA!H29:M29))</f>
-        <v>17342979461.645</v>
+        <v>17349270072.654999</v>
       </c>
       <c r="I29" t="b">
         <f>A29=IPVA!A29</f>
@@ -11383,11 +11479,29 @@
       <c r="J29" s="9"/>
       <c r="K29" s="93">
         <f t="shared" si="0"/>
-        <v>1.0399214240768544</v>
+        <v>1.041075511593281</v>
       </c>
       <c r="L29" s="9">
         <f t="shared" si="1"/>
-        <v>-7155390260.8175354</v>
+        <v>-7166840819.0249939</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E30" s="9" t="b">
+        <f>E29/0.75=SUM(ICMS!B29:G29)</f>
+        <v>1</v>
+      </c>
+      <c r="F30" s="9" t="b">
+        <f>F29/0.5=SUM(IPVA!B29:G29)</f>
+        <v>1</v>
+      </c>
+      <c r="G30" s="9" t="b">
+        <f>G29/0.75=SUM(ICMS!H29:M29)</f>
+        <v>1</v>
+      </c>
+      <c r="H30" t="b">
+        <f>H29/0.5=SUM(IPVA!H29:M29)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
@@ -11506,7 +11620,7 @@
       </c>
       <c r="G33" s="4">
         <f>0.75*VLOOKUP($A$32,ICMS!$A$2:$M$29,Planilha1!G31,0)</f>
-        <v>29823779561.355</v>
+        <v>29954298740.924995</v>
       </c>
       <c r="H33" s="4">
         <f>0.75*VLOOKUP($A$32,ICMS!$A$2:$M$29,Planilha1!H31,0)</f>
@@ -11526,11 +11640,11 @@
       </c>
       <c r="L33" s="4">
         <f>0.75*VLOOKUP($A$32,ICMS!$A$2:$M$29,Planilha1!L31,0)</f>
-        <v>23632179018.255005</v>
+        <v>23633169054.015003</v>
       </c>
       <c r="M33" s="4">
         <f>0.75*VLOOKUP($A$32,ICMS!$A$2:$M$29,Planilha1!M31,0)</f>
-        <v>27033569410.492493</v>
+        <v>27145357385.084999</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
@@ -11579,11 +11693,11 @@
       </c>
       <c r="L34" s="4">
         <f>0.5*VLOOKUP($A$32,IPVA!$A$2:$M$29,Planilha1!L31,0)</f>
-        <v>1037965505.4949999</v>
+        <v>1037978767.395</v>
       </c>
       <c r="M34" s="4">
         <f>0.5*VLOOKUP($A$32,IPVA!$A$2:$M$29,Planilha1!M31,0)</f>
-        <v>1297432702.7849998</v>
+        <v>1303710051.895</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
@@ -11617,7 +11731,7 @@
       </c>
       <c r="G38" s="97">
         <f t="shared" si="3"/>
-        <v>30907697822.044998</v>
+        <v>31038217001.614994</v>
       </c>
       <c r="H38" s="97">
         <f t="shared" si="3"/>
@@ -11637,11 +11751,11 @@
       </c>
       <c r="L38" s="97">
         <f t="shared" si="3"/>
-        <v>24670144523.750004</v>
+        <v>24671147821.410004</v>
       </c>
       <c r="M38" s="97">
         <f t="shared" si="3"/>
-        <v>28331002113.277493</v>
+        <v>28449067436.98</v>
       </c>
       <c r="N38" s="97"/>
     </row>
@@ -11700,11 +11814,11 @@
       </c>
       <c r="L40" s="98">
         <f t="shared" si="4"/>
-        <v>26214104925.010002</v>
+        <v>26215108222.670002</v>
       </c>
       <c r="M40" s="98">
         <f t="shared" si="4"/>
-        <v>39124962514.537491</v>
+        <v>39243027838.240005</v>
       </c>
       <c r="N40" s="98">
         <f t="shared" si="4"/>

</xml_diff>